<commit_message>
Revert "perf(size): Optimize output size by removing unecessary stuff"
This reverts commit 6dc952afe37f358368038792972eaddd3b2b84e2.
Excel complains about these missing parts, while Numbers is not.
</commit_message>
<xml_diff>
--- a/test/resources/empty-file.xlsx
+++ b/test/resources/empty-file.xlsx
@@ -1,44 +1,85 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="1" lowestEdited="1" rupBuild="9000"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
+  </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="200" formatCode="yyyy-mm-dd"/>
     <numFmt numFmtId="201" formatCode="yyyy-mm-dd hh:mm:ss"/>
   </numFmts>
+  <fonts count="1" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="2">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+  </fills>
+  <borders count="1">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+  </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" xfId="0"/>
-    <xf numFmtId="1" xfId="0"/>
-    <xf numFmtId="2" xfId="0"/>
-    <xf numFmtId="3" xfId="0"/>
-    <xf numFmtId="4" xfId="0"/>
-    <xf numFmtId="11" xfId="0"/>
-    <xf numFmtId="49" xfId="0"/>
-    <xf numFmtId="200" xfId="0"/>
-    <xf numFmtId="201" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="200" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="201" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr baseColWidth="30" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>